<commit_message>
Update Sidebar Pasien and Pendaftaran
</commit_message>
<xml_diff>
--- a/public/source_download/cobadownload.xlsx
+++ b/public/source_download/cobadownload.xlsx
@@ -1,19 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bintang Vet Clinic\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Belajar Laravel\bintang-vet-clinic\public\source_download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5181874-78BC-40CB-838E-5595A31B2058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70DAE6B-C47C-48A0-A038-3C0FB093CD09}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87BEA1B2-1379-4E57-B5FA-A3A6CE3B9F95}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Daftar Satuan Barang" sheetId="2" r:id="rId2"/>
+    <sheet name="Daftar Kategori Barang" sheetId="3" r:id="rId3"/>
+    <sheet name="Daftar Cabang" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,9 +37,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
-    <t>test12345</t>
+    <t>Daftar Barang</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Satuan Barang</t>
+  </si>
+  <si>
+    <t>Kategori Barang</t>
+  </si>
+  <si>
+    <t>Daftar Cabang</t>
   </si>
 </sst>
 </file>
@@ -394,10 +409,94 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B73323F-39EB-46D3-B693-08BE2DED2BE6}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477D07F2-1ED8-4E11-BF70-8DED84BC1AEB}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD64DC39-D407-4894-B16B-746CDBAA734A}">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>